<commit_message>
the files are updated and results attached
</commit_message>
<xml_diff>
--- a/RL algorithms/plot.xlsx
+++ b/RL algorithms/plot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mahdi\Desktop\RL project github\RL algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05185C18-E342-4C53-B62D-6B9124A9EC25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A44221-DAC3-46C6-8FE3-CE49F02898FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>SAC</t>
   </si>
@@ -48,18 +48,6 @@
   </si>
   <si>
     <t>TSAC</t>
-  </si>
-  <si>
-    <t>SAC-edited</t>
-  </si>
-  <si>
-    <t>PPO-edited</t>
-  </si>
-  <si>
-    <t>TD3-edited</t>
-  </si>
-  <si>
-    <t>TSAC-edited</t>
   </si>
 </sst>
 </file>
@@ -95,8 +83,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -130,7 +121,17 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14241447944006999"/>
+          <c:y val="4.6594971558722872E-2"/>
+          <c:w val="0.68711307961504808"/>
+          <c:h val="0.80344700060463392"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -154,7 +155,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$101</c:f>
+              <c:f>Sheet1!$A$2:$A$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -463,7 +464,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$101</c:f>
+              <c:f>Sheet1!$B$2:$B$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -762,10 +763,10 @@
                   <c:v>49.695613054404902</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>155.721625773461</c:v>
+                  <c:v>98.273650000000004</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>148.091289730798</c:v>
+                  <c:v>96.568929999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -797,7 +798,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$101</c:f>
+              <c:f>Sheet1!$A$2:$A$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -1106,7 +1107,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$101</c:f>
+              <c:f>Sheet1!$C$2:$C$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -1440,7 +1441,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$101</c:f>
+              <c:f>Sheet1!$A$2:$A$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -1749,7 +1750,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$101</c:f>
+              <c:f>Sheet1!$D$2:$D$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -2072,7 +2073,7 @@
           <c:spPr>
             <a:ln w="9525" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="00B050"/>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -2083,7 +2084,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$101</c:f>
+              <c:f>Sheet1!$A$2:$A$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -2392,7 +2393,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$101</c:f>
+              <c:f>Sheet1!$E$2:$E$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -2762,6 +2763,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.42800568678915135"/>
+              <c:y val="0.9208582573627393"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2950,7 +2959,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.81797200349956256"/>
+          <c:x val="0.8318608923884514"/>
           <c:y val="0.24955092720324507"/>
           <c:w val="0.13480577427821522"/>
           <c:h val="0.31451825935861843"/>
@@ -3549,16 +3558,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>83820</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>118110</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>312421</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>112248</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>388620</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>118110</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>112249</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3849,10 +3858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I101"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3863,3328 +3872,1718 @@
     <col min="9" max="9" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>-10.1766220458723</v>
+      </c>
+      <c r="C2" s="1">
+        <v>-94.458730000000003</v>
+      </c>
+      <c r="D2" s="1">
+        <v>-4.9063917251197999</v>
+      </c>
+      <c r="E2" s="1">
+        <v>-23.124741675653123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1.1851810404029699</v>
+      </c>
+      <c r="C3" s="1">
+        <v>-101.322</v>
+      </c>
+      <c r="D3" s="1">
+        <v>-2.4792537809804003</v>
+      </c>
+      <c r="E3" s="1">
+        <v>-6.1840695420235203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>11.0213197310214</v>
+      </c>
+      <c r="C4" s="1">
+        <v>-85.937899999999999</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3.1652213447603099</v>
+      </c>
+      <c r="E4" s="1">
+        <v>-32.289477626153435</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.3402271453255701</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-64.482709999999997</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4.27800517005132</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3.1539638189797219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B6" s="1">
+        <v>-0.122709280489072</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2.3190279999999999</v>
+      </c>
+      <c r="D6" s="1">
+        <v>4.2592190461731603</v>
+      </c>
+      <c r="E6" s="1">
+        <v>-13.051865992099801</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="B7" s="1">
+        <v>16.8872645259904</v>
+      </c>
+      <c r="C7" s="1">
+        <v>-27.128245172742599</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3.3226311322287296</v>
+      </c>
+      <c r="E7" s="1">
+        <v>-33.153300743451837</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="B8" s="1">
+        <v>17.043504809856699</v>
+      </c>
+      <c r="C8" s="1">
+        <v>-73.205113999999995</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3.2209705863673399</v>
+      </c>
+      <c r="E8" s="1">
+        <v>8.5678119963610602</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>-10.1766220458723</v>
-      </c>
-      <c r="B2">
-        <v>-421.80346001431502</v>
-      </c>
-      <c r="C2">
-        <v>-14.9063917251198</v>
-      </c>
-      <c r="D2">
-        <v>-7.2264817736416003</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <f>A2</f>
-        <v>-10.1766220458723</v>
-      </c>
-      <c r="G2">
-        <v>-94.458730000000003</v>
-      </c>
-      <c r="H2">
-        <f>SUM(C2,10)</f>
-        <v>-4.9063917251197999</v>
-      </c>
-      <c r="I2">
-        <f>D2*3.2</f>
-        <v>-23.124741675653123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>1.1851810404029699</v>
-      </c>
-      <c r="B3">
-        <v>-529.19004955298897</v>
-      </c>
-      <c r="C3">
-        <v>-12.4792537809804</v>
-      </c>
-      <c r="D3">
-        <v>-1.93252173188235</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F66" si="0">A3</f>
-        <v>1.1851810404029699</v>
-      </c>
-      <c r="G3">
-        <f>-101.322</f>
-        <v>-101.322</v>
-      </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H66" si="1">SUM(C3,10)</f>
-        <v>-2.4792537809804003</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I5" si="2">D3*3.2</f>
-        <v>-6.1840695420235203</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>11.0213197310214</v>
-      </c>
-      <c r="B4">
-        <v>-223.80220221317299</v>
-      </c>
-      <c r="C4">
-        <v>-6.8347786552396901</v>
-      </c>
-      <c r="D4">
-        <v>-5.7659781475273997</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="0"/>
-        <v>11.0213197310214</v>
-      </c>
-      <c r="G4">
-        <f>-85.9379</f>
-        <v>-85.937899999999999</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="1"/>
-        <v>3.1652213447603099</v>
-      </c>
-      <c r="I4">
-        <f>D4*5.6</f>
-        <v>-32.289477626153435</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>1.3402271453255701</v>
-      </c>
-      <c r="B5">
-        <v>-418.60203594644298</v>
-      </c>
-      <c r="C5">
-        <v>-5.72199482994868</v>
-      </c>
-      <c r="D5">
-        <v>0.98561369343116301</v>
-      </c>
-      <c r="E5">
-        <v>3</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="0"/>
-        <v>1.3402271453255701</v>
-      </c>
-      <c r="G5">
-        <f>-64.48271</f>
-        <v>-64.482709999999997</v>
-      </c>
-      <c r="H5">
-        <f t="shared" si="1"/>
-        <v>4.27800517005132</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="2"/>
-        <v>3.1539638189797219</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>-0.122709280489072</v>
-      </c>
-      <c r="B6">
-        <v>22.6827763151204</v>
-      </c>
-      <c r="C6">
-        <v>-5.7407809538268397</v>
-      </c>
-      <c r="D6">
-        <v>-13.051865992099801</v>
-      </c>
-      <c r="E6">
-        <v>4</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
-        <v>-0.122709280489072</v>
-      </c>
-      <c r="G6">
-        <f>2.319028</f>
-        <v>2.3190279999999999</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="1"/>
-        <v>4.2592190461731603</v>
-      </c>
-      <c r="I6">
-        <f>D6</f>
-        <v>-13.051865992099801</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>16.8872645259904</v>
-      </c>
-      <c r="B7">
-        <v>-27.128245172742599</v>
-      </c>
-      <c r="C7">
-        <v>-6.6773688677712704</v>
-      </c>
-      <c r="D7">
-        <v>13.8138753097716</v>
-      </c>
-      <c r="E7">
-        <v>5</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="0"/>
-        <v>16.8872645259904</v>
-      </c>
-      <c r="G7">
-        <f>B7</f>
-        <v>-27.128245172742599</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="1"/>
-        <v>3.3226311322287296</v>
-      </c>
-      <c r="I7">
-        <f>D7*(-2.4)</f>
-        <v>-33.153300743451837</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>17.043504809856699</v>
-      </c>
-      <c r="B8">
-        <v>-386.76426823900999</v>
-      </c>
-      <c r="C8">
-        <v>-6.7790294136326601</v>
-      </c>
-      <c r="D8">
-        <v>8.5678119963610602</v>
-      </c>
-      <c r="E8">
-        <v>6</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>17.043504809856699</v>
-      </c>
-      <c r="G8">
-        <f>-73.205114</f>
-        <v>-73.205113999999995</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="1"/>
-        <v>3.2209705863673399</v>
-      </c>
-      <c r="I8">
-        <f t="shared" ref="I3:I66" si="3">D8</f>
-        <v>8.5678119963610602</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="B9" s="1">
         <v>-27.198355425911899</v>
       </c>
-      <c r="B9">
+      <c r="C9" s="1">
         <v>-34.994460061197302</v>
       </c>
-      <c r="C9">
-        <v>-6.6594635102928104</v>
-      </c>
-      <c r="D9">
+      <c r="D9" s="1">
+        <v>3.3405364897071896</v>
+      </c>
+      <c r="E9" s="1">
         <v>19.342997748423901</v>
       </c>
-      <c r="E9">
-        <v>7</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>-27.198355425911899</v>
-      </c>
-      <c r="G9">
-        <f>B9</f>
-        <v>-34.994460061197302</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="1"/>
-        <v>3.3405364897071896</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="3"/>
-        <v>19.342997748423901</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
         <v>88.748709382042094</v>
       </c>
-      <c r="B10">
+      <c r="C10" s="1">
         <v>80.091695837580303</v>
       </c>
-      <c r="C10">
-        <v>-5.72565633936195</v>
-      </c>
-      <c r="D10">
-        <v>3.4225974489054201</v>
-      </c>
-      <c r="E10">
-        <v>8</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="0"/>
-        <v>88.748709382042094</v>
-      </c>
-      <c r="G10">
-        <f t="shared" ref="G3:G66" si="4">B10</f>
-        <v>80.091695837580303</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="1"/>
+      <c r="D10" s="1">
         <v>4.27434366063805</v>
       </c>
-      <c r="I10">
-        <f>D10+8</f>
+      <c r="E10" s="1">
         <v>11.422597448905421</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
         <v>-1.0873343904319599</v>
       </c>
-      <c r="B11">
+      <c r="C11" s="1">
         <v>35.604778953818801</v>
       </c>
-      <c r="C11">
-        <v>-5.2237581226338099</v>
-      </c>
-      <c r="D11">
+      <c r="D11" s="1">
+        <v>4.7762418773661901</v>
+      </c>
+      <c r="E11" s="1">
         <v>13.082881068782299</v>
       </c>
-      <c r="E11">
-        <v>9</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="0"/>
-        <v>-1.0873343904319599</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="4"/>
-        <v>35.604778953818801</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="1"/>
-        <v>4.7762418773661901</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="3"/>
-        <v>13.082881068782299</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
         <v>1.7792711802708701</v>
       </c>
-      <c r="B12">
+      <c r="C12" s="1">
         <v>13.1367426093804</v>
       </c>
-      <c r="C12">
-        <v>-5.8081800572383999</v>
-      </c>
-      <c r="D12">
-        <v>3.8838138649025602</v>
-      </c>
-      <c r="E12">
-        <v>10</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>1.7792711802708701</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="4"/>
-        <v>13.1367426093804</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="1"/>
+      <c r="D12" s="1">
         <v>4.1918199427616001</v>
       </c>
-      <c r="I12">
-        <f>D12+3</f>
+      <c r="E12" s="1">
         <v>6.8838138649025602</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
         <v>-47.181786289104302</v>
       </c>
-      <c r="B13">
-        <v>-72.624589010773803</v>
-      </c>
-      <c r="C13">
-        <v>-6.6670577188575804</v>
-      </c>
-      <c r="D13">
-        <v>5.9282670926167897</v>
-      </c>
-      <c r="E13">
-        <v>11</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>-47.181786289104302</v>
-      </c>
-      <c r="G13">
-        <f>-58.8463</f>
+      <c r="C13" s="1">
         <v>-58.846299999999999</v>
       </c>
-      <c r="H13">
-        <f>SUM(C13,11.5)</f>
+      <c r="D13" s="1">
         <v>4.8329422811424196</v>
       </c>
-      <c r="I13">
-        <f>D13+7</f>
+      <c r="E13" s="1">
         <v>12.928267092616789</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1">
         <v>-6.1268286958602802</v>
       </c>
-      <c r="B14">
+      <c r="C14" s="1">
         <v>22.204472763959402</v>
       </c>
-      <c r="C14">
-        <v>-6.8498027398330503</v>
-      </c>
-      <c r="D14">
-        <v>9.00001956162175</v>
-      </c>
-      <c r="E14">
-        <v>12</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="0"/>
-        <v>-6.1268286958602802</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="4"/>
-        <v>22.204472763959402</v>
-      </c>
-      <c r="H14">
-        <f t="shared" ref="H14:H31" si="5">SUM(C14,11.5)</f>
+      <c r="D14" s="1">
         <v>4.6501972601669497</v>
       </c>
-      <c r="I14">
-        <f t="shared" ref="I14:I15" si="6">D14+7</f>
+      <c r="E14" s="1">
         <v>16.000019561621748</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
         <v>-11.5777737459976</v>
       </c>
-      <c r="B15">
+      <c r="C15" s="1">
         <v>17.059128726242101</v>
       </c>
-      <c r="C15">
-        <v>-6.7248637920158902</v>
-      </c>
-      <c r="D15">
-        <v>2.6874153727222998</v>
-      </c>
-      <c r="E15">
-        <v>13</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="0"/>
-        <v>-11.5777737459976</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="4"/>
-        <v>17.059128726242101</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="5"/>
+      <c r="D15" s="1">
         <v>4.7751362079841098</v>
       </c>
-      <c r="I15">
-        <f t="shared" si="6"/>
+      <c r="E15" s="1">
         <v>9.6874153727222989</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
         <v>-3.9196477633414899</v>
       </c>
-      <c r="B16">
-        <v>-168.332523811427</v>
-      </c>
-      <c r="C16">
-        <v>-6.2654939285304998</v>
-      </c>
-      <c r="D16">
+      <c r="C16" s="1">
+        <v>-46.392069999999997</v>
+      </c>
+      <c r="D16" s="1">
+        <v>5.2345060714695002</v>
+      </c>
+      <c r="E16" s="1">
         <v>-14.499335277683199</v>
       </c>
-      <c r="E16">
-        <v>14</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="0"/>
-        <v>-3.9196477633414899</v>
-      </c>
-      <c r="G16">
-        <f>-46.39207</f>
-        <v>-46.392069999999997</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="5"/>
-        <v>5.2345060714695002</v>
-      </c>
-      <c r="I16">
-        <f>D16</f>
-        <v>-14.499335277683199</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1">
         <v>23.3037635801923</v>
       </c>
-      <c r="B17">
+      <c r="C17" s="1">
         <v>34.245550687394498</v>
       </c>
-      <c r="C17">
-        <v>-5.9248260622603102</v>
-      </c>
-      <c r="D17">
-        <v>-2.3547091774235498</v>
-      </c>
-      <c r="E17">
-        <v>15</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="0"/>
-        <v>23.3037635801923</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="4"/>
-        <v>34.245550687394498</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="5"/>
+      <c r="D17" s="1">
         <v>5.5751739377396898</v>
       </c>
-      <c r="I17">
-        <f>D17*2</f>
+      <c r="E17" s="1">
         <v>-4.7094183548470996</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1">
         <v>-0.82575321838866</v>
       </c>
-      <c r="B18">
+      <c r="C18" s="1">
         <v>28.003502563835301</v>
       </c>
-      <c r="C18">
-        <v>-6.23241826075422</v>
-      </c>
-      <c r="D18">
+      <c r="D18" s="1">
+        <v>5.26758173924578</v>
+      </c>
+      <c r="E18" s="1">
         <v>-15.747760980164699</v>
       </c>
-      <c r="E18">
-        <v>16</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="0"/>
-        <v>-0.82575321838866</v>
-      </c>
-      <c r="G18">
-        <f t="shared" si="4"/>
-        <v>28.003502563835301</v>
-      </c>
-      <c r="H18">
-        <f t="shared" si="5"/>
-        <v>5.26758173924578</v>
-      </c>
-      <c r="I18">
-        <f>D18</f>
-        <v>-15.747760980164699</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1">
         <v>-42.498481630852197</v>
       </c>
-      <c r="B19">
+      <c r="C19" s="1">
         <v>3.0587572304970201</v>
       </c>
-      <c r="C19">
-        <v>-5.9145190700421697</v>
-      </c>
-      <c r="D19">
+      <c r="D19" s="1">
+        <v>5.5854809299578303</v>
+      </c>
+      <c r="E19" s="1">
         <v>5.5561181363275596</v>
       </c>
-      <c r="E19">
-        <v>17</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="0"/>
-        <v>-42.498481630852197</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="4"/>
-        <v>3.0587572304970201</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="5"/>
-        <v>5.5854809299578303</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="3"/>
-        <v>5.5561181363275596</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1">
         <v>17.6863496879308</v>
       </c>
-      <c r="B20">
+      <c r="C20" s="1">
         <v>39.820322551481802</v>
       </c>
-      <c r="C20">
-        <v>-6.4273730267051503</v>
-      </c>
-      <c r="D20">
+      <c r="D20" s="1">
+        <v>5.0726269732948497</v>
+      </c>
+      <c r="E20" s="1">
         <v>2.9883257192301298</v>
       </c>
-      <c r="E20">
-        <v>18</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="0"/>
-        <v>17.6863496879308</v>
-      </c>
-      <c r="G20">
-        <f t="shared" si="4"/>
-        <v>39.820322551481802</v>
-      </c>
-      <c r="H20">
-        <f t="shared" si="5"/>
-        <v>5.0726269732948497</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="3"/>
-        <v>2.9883257192301298</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1">
         <v>25.8684555083323</v>
       </c>
-      <c r="B21">
+      <c r="C21" s="1">
         <v>29.486793046953601</v>
       </c>
-      <c r="C21">
-        <v>-5.9773300711479296</v>
-      </c>
-      <c r="D21">
+      <c r="D21" s="1">
+        <v>5.5226699288520704</v>
+      </c>
+      <c r="E21" s="1">
         <v>9.8268060023553794</v>
       </c>
-      <c r="E21">
-        <v>19</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="0"/>
-        <v>25.8684555083323</v>
-      </c>
-      <c r="G21">
-        <f t="shared" si="4"/>
-        <v>29.486793046953601</v>
-      </c>
-      <c r="H21">
-        <f t="shared" si="5"/>
-        <v>5.5226699288520704</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="3"/>
-        <v>9.8268060023553794</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1">
         <v>-15.3585551863459</v>
       </c>
-      <c r="B22">
+      <c r="C22" s="1">
         <v>-37.539009123413301</v>
       </c>
-      <c r="C22">
-        <v>-5.8653129826858903</v>
-      </c>
-      <c r="D22">
+      <c r="D22" s="1">
+        <v>5.6346870173141097</v>
+      </c>
+      <c r="E22" s="1">
         <v>6.85188854439241</v>
       </c>
-      <c r="E22">
-        <v>20</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="0"/>
-        <v>-15.3585551863459</v>
-      </c>
-      <c r="G22">
-        <f t="shared" si="4"/>
-        <v>-37.539009123413301</v>
-      </c>
-      <c r="H22">
-        <f t="shared" si="5"/>
-        <v>5.6346870173141097</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="3"/>
-        <v>6.85188854439241</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1">
         <v>30.693178809471899</v>
       </c>
-      <c r="B23">
+      <c r="C23" s="1">
         <v>-83.716319068388401</v>
       </c>
-      <c r="C23">
-        <v>-6.0528322694824297</v>
-      </c>
-      <c r="D23">
-        <v>8.6684054667238897</v>
-      </c>
-      <c r="E23">
-        <v>21</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="0"/>
-        <v>30.693178809471899</v>
-      </c>
-      <c r="G23">
-        <f t="shared" si="4"/>
-        <v>-83.716319068388401</v>
-      </c>
-      <c r="H23">
-        <f t="shared" si="5"/>
+      <c r="D23" s="1">
         <v>5.4471677305175703</v>
       </c>
-      <c r="I23">
-        <f>D23+20</f>
+      <c r="E23" s="1">
         <v>28.66840546672389</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1">
         <v>-29.911443127588502</v>
       </c>
-      <c r="B24">
+      <c r="C24" s="1">
         <v>-30.513575296143902</v>
       </c>
-      <c r="C24">
-        <v>-5.5876373668279697</v>
-      </c>
-      <c r="D24">
-        <v>0.25064301627466701</v>
-      </c>
-      <c r="E24">
-        <v>22</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="0"/>
-        <v>-29.911443127588502</v>
-      </c>
-      <c r="G24">
-        <f t="shared" si="4"/>
-        <v>-30.513575296143902</v>
-      </c>
-      <c r="H24">
-        <f t="shared" si="5"/>
+      <c r="D24" s="1">
         <v>5.9123626331720303</v>
       </c>
-      <c r="I24">
-        <f>D24+20</f>
+      <c r="E24" s="1">
         <v>20.250643016274665</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1">
         <v>27.698765240846502</v>
       </c>
-      <c r="B25">
+      <c r="C25" s="1">
         <v>-92.700817770484903</v>
       </c>
-      <c r="C25">
-        <v>-5.8913853516274699</v>
-      </c>
-      <c r="D25">
-        <v>15.1907755354503</v>
-      </c>
-      <c r="E25">
-        <v>23</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="0"/>
-        <v>27.698765240846502</v>
-      </c>
-      <c r="G25">
-        <f t="shared" si="4"/>
-        <v>-92.700817770484903</v>
-      </c>
-      <c r="H25">
-        <f t="shared" si="5"/>
+      <c r="D25" s="1">
         <v>5.6086146483725301</v>
       </c>
-      <c r="I25">
-        <f>D25+38</f>
+      <c r="E25" s="1">
         <v>53.1907755354503</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1">
         <v>12.746315018485699</v>
       </c>
-      <c r="B26">
+      <c r="C26" s="1">
         <v>4.1780589164727404</v>
       </c>
-      <c r="C26">
-        <v>-5.8700002019420801</v>
-      </c>
-      <c r="D26">
-        <v>0.459279928126271</v>
-      </c>
-      <c r="E26">
-        <v>24</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="0"/>
-        <v>12.746315018485699</v>
-      </c>
-      <c r="G26">
-        <f t="shared" si="4"/>
-        <v>4.1780589164727404</v>
-      </c>
-      <c r="H26">
-        <f t="shared" si="5"/>
+      <c r="D26" s="1">
         <v>5.6299997980579199</v>
       </c>
-      <c r="I26">
-        <f>D26+20</f>
+      <c r="E26" s="1">
         <v>20.459279928126271</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" s="1">
         <v>-51.407929927760101</v>
       </c>
-      <c r="B27">
+      <c r="C27" s="1">
         <v>34.157566009762597</v>
       </c>
-      <c r="C27">
-        <v>-5.8514058540146801</v>
-      </c>
-      <c r="D27">
-        <v>9.7654878119851904</v>
-      </c>
-      <c r="E27">
-        <v>25</v>
-      </c>
-      <c r="F27">
-        <f t="shared" si="0"/>
-        <v>-51.407929927760101</v>
-      </c>
-      <c r="G27">
-        <f t="shared" si="4"/>
-        <v>34.157566009762597</v>
-      </c>
-      <c r="H27">
-        <f t="shared" si="5"/>
+      <c r="D27" s="1">
         <v>5.6485941459853199</v>
       </c>
-      <c r="I27">
-        <f>D27+28</f>
+      <c r="E27" s="1">
         <v>37.765487811985189</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" s="1">
         <v>4.4462490282357701</v>
       </c>
-      <c r="B28">
-        <v>-205.01881517869001</v>
-      </c>
-      <c r="C28">
-        <v>-5.6589760680154102</v>
-      </c>
-      <c r="D28">
-        <v>1.6315090256526701</v>
-      </c>
-      <c r="E28">
-        <v>26</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="0"/>
-        <v>4.4462490282357701</v>
-      </c>
-      <c r="G28">
-        <f>-67.10336</f>
+      <c r="C28" s="1">
         <v>-67.103359999999995</v>
       </c>
-      <c r="H28">
-        <f t="shared" si="5"/>
+      <c r="D28" s="1">
         <v>5.8410239319845898</v>
       </c>
-      <c r="I28">
-        <f>D28+16</f>
+      <c r="E28" s="1">
         <v>17.631509025652669</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" s="1">
         <v>3.2375772830097498</v>
       </c>
-      <c r="B29">
+      <c r="C29" s="1">
         <v>47.355020219267203</v>
       </c>
-      <c r="C29">
-        <v>-6.6983161210502704</v>
-      </c>
-      <c r="D29">
+      <c r="D29" s="1">
+        <v>4.8016838789497296</v>
+      </c>
+      <c r="E29" s="1">
         <v>11.807317708194899</v>
       </c>
-      <c r="E29">
-        <v>27</v>
-      </c>
-      <c r="F29">
-        <f t="shared" si="0"/>
-        <v>3.2375772830097498</v>
-      </c>
-      <c r="G29">
-        <f t="shared" si="4"/>
-        <v>47.355020219267203</v>
-      </c>
-      <c r="H29">
-        <f t="shared" si="5"/>
-        <v>4.8016838789497296</v>
-      </c>
-      <c r="I29">
-        <f t="shared" si="3"/>
-        <v>11.807317708194899</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" s="1">
         <v>15.0445345542817</v>
       </c>
-      <c r="B30">
+      <c r="C30" s="1">
         <v>0.71659565553576998</v>
       </c>
-      <c r="C30">
-        <v>-5.2571834297214197</v>
-      </c>
-      <c r="D30">
-        <v>2.9790470586525402</v>
-      </c>
-      <c r="E30">
-        <v>28</v>
-      </c>
-      <c r="F30">
-        <f t="shared" si="0"/>
-        <v>15.0445345542817</v>
-      </c>
-      <c r="G30">
-        <f t="shared" si="4"/>
-        <v>0.71659565553576998</v>
-      </c>
-      <c r="H30">
-        <f t="shared" si="5"/>
+      <c r="D30" s="1">
         <v>6.2428165702785803</v>
       </c>
-      <c r="I30">
-        <f>D30*3+28</f>
+      <c r="E30" s="1">
         <v>36.93714117595762</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" s="1">
         <v>7.3293608184331198</v>
       </c>
-      <c r="B31">
+      <c r="C31" s="1">
         <v>73.468005107911907</v>
       </c>
-      <c r="C31">
-        <v>-6.1871391389323396</v>
-      </c>
-      <c r="D31">
-        <v>6.7911772172185696</v>
-      </c>
-      <c r="E31">
-        <v>29</v>
-      </c>
-      <c r="F31">
-        <f t="shared" si="0"/>
-        <v>7.3293608184331198</v>
-      </c>
-      <c r="G31">
-        <f t="shared" si="4"/>
-        <v>73.468005107911907</v>
-      </c>
-      <c r="H31">
-        <f>SUM(C31,11.5)</f>
+      <c r="D31" s="1">
         <v>5.3128608610676604</v>
       </c>
-      <c r="I31">
-        <f t="shared" ref="I31:I36" si="7">D31*3+6</f>
+      <c r="E31" s="1">
         <v>26.373531651655711</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" s="1">
         <v>-4.4377838978797</v>
       </c>
-      <c r="B32">
+      <c r="C32" s="1">
         <v>16.5942282535526</v>
       </c>
-      <c r="C32">
-        <v>-6.4821569272892203</v>
-      </c>
-      <c r="D32">
-        <v>11.343829415080201</v>
-      </c>
-      <c r="E32">
-        <v>30</v>
-      </c>
-      <c r="F32">
-        <f t="shared" si="0"/>
-        <v>-4.4377838978797</v>
-      </c>
-      <c r="G32">
-        <f t="shared" si="4"/>
-        <v>16.5942282535526</v>
-      </c>
-      <c r="H32">
-        <f>SUM(C32,10)</f>
+      <c r="D32" s="1">
         <v>3.5178430727107797</v>
       </c>
-      <c r="I32">
-        <f t="shared" si="7"/>
+      <c r="E32" s="1">
         <v>40.031488245240602</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" s="1">
         <v>13.207744573998299</v>
       </c>
-      <c r="B33">
+      <c r="C33" s="1">
         <v>15.250149637224</v>
       </c>
-      <c r="C33">
-        <v>-6.8813861184831397</v>
-      </c>
-      <c r="D33">
-        <v>5.9970030416814399</v>
-      </c>
-      <c r="E33">
-        <v>31</v>
-      </c>
-      <c r="F33">
-        <f t="shared" si="0"/>
-        <v>13.207744573998299</v>
-      </c>
-      <c r="G33">
-        <f t="shared" si="4"/>
-        <v>15.250149637224</v>
-      </c>
-      <c r="H33">
-        <f t="shared" si="1"/>
+      <c r="D33" s="1">
         <v>3.1186138815168603</v>
       </c>
-      <c r="I33">
-        <f t="shared" si="7"/>
+      <c r="E33" s="1">
         <v>23.991009125044322</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" s="1">
         <v>-18.677482487078901</v>
       </c>
-      <c r="B34">
+      <c r="C34" s="1">
         <v>45.831401130652502</v>
       </c>
-      <c r="C34">
-        <v>-5.8797230598400798</v>
-      </c>
-      <c r="D34">
-        <v>6.8338415314100596</v>
-      </c>
-      <c r="E34">
-        <v>32</v>
-      </c>
-      <c r="F34">
-        <f t="shared" si="0"/>
-        <v>-18.677482487078901</v>
-      </c>
-      <c r="G34">
-        <f t="shared" si="4"/>
-        <v>45.831401130652502</v>
-      </c>
-      <c r="H34">
-        <f t="shared" si="1"/>
+      <c r="D34" s="1">
         <v>4.1202769401599202</v>
       </c>
-      <c r="I34">
-        <f t="shared" si="7"/>
+      <c r="E34" s="1">
         <v>26.50152459423018</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" s="1">
         <v>18.767209785226399</v>
       </c>
-      <c r="B35">
+      <c r="C35" s="1">
         <v>18.235268982237098</v>
       </c>
-      <c r="C35">
-        <v>-5.9388351774287402</v>
-      </c>
-      <c r="D35">
-        <v>4.6714473667448502</v>
-      </c>
-      <c r="E35">
-        <v>33</v>
-      </c>
-      <c r="F35">
-        <f t="shared" si="0"/>
-        <v>18.767209785226399</v>
-      </c>
-      <c r="G35">
-        <f t="shared" si="4"/>
-        <v>18.235268982237098</v>
-      </c>
-      <c r="H35">
-        <f t="shared" si="1"/>
+      <c r="D35" s="1">
         <v>4.0611648225712598</v>
       </c>
-      <c r="I35">
-        <f>D35*3+26</f>
+      <c r="E35" s="1">
         <v>40.014342100234551</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" s="1">
         <v>63.918850908294203</v>
       </c>
-      <c r="B36">
+      <c r="C36" s="1">
         <v>29.8855217502622</v>
       </c>
-      <c r="C36">
-        <v>-6.9119608038599401</v>
-      </c>
-      <c r="D36">
-        <v>7.6144942593264</v>
-      </c>
-      <c r="E36">
-        <v>34</v>
-      </c>
-      <c r="F36">
-        <f t="shared" si="0"/>
-        <v>63.918850908294203</v>
-      </c>
-      <c r="G36">
-        <f t="shared" si="4"/>
-        <v>29.8855217502622</v>
-      </c>
-      <c r="H36">
-        <f t="shared" si="1"/>
+      <c r="D36" s="1">
         <v>3.0880391961400599</v>
       </c>
-      <c r="I36">
-        <f t="shared" si="7"/>
+      <c r="E36" s="1">
         <v>28.843482777979201</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" s="1">
         <v>12.8308466226874</v>
       </c>
-      <c r="B37">
+      <c r="C37" s="1">
         <v>41.972979686594599</v>
       </c>
-      <c r="C37">
-        <v>-6.6870724451924799</v>
-      </c>
-      <c r="D37">
-        <v>1.9433717759706499</v>
-      </c>
-      <c r="E37">
-        <v>35</v>
-      </c>
-      <c r="F37">
-        <f t="shared" si="0"/>
-        <v>12.8308466226874</v>
-      </c>
-      <c r="G37">
-        <f t="shared" si="4"/>
-        <v>41.972979686594599</v>
-      </c>
-      <c r="H37">
-        <f>SUM(C37,12)</f>
+      <c r="D37" s="1">
         <v>5.3129275548075201</v>
       </c>
-      <c r="I37">
-        <f>D37+46</f>
+      <c r="E37" s="1">
         <v>47.943371775970647</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" s="1">
         <v>6.1225908422137598E-2</v>
       </c>
-      <c r="B38">
+      <c r="C38" s="1">
         <v>44.493335469931303</v>
       </c>
-      <c r="C38">
-        <v>-6.7473158211883097</v>
-      </c>
-      <c r="D38">
-        <v>6.5209300423012202</v>
-      </c>
-      <c r="E38">
-        <v>36</v>
-      </c>
-      <c r="F38">
-        <f t="shared" si="0"/>
-        <v>6.1225908422137598E-2</v>
-      </c>
-      <c r="G38">
-        <f t="shared" si="4"/>
-        <v>44.493335469931303</v>
-      </c>
-      <c r="H38">
-        <f t="shared" ref="H38:H43" si="8">SUM(C38,12)</f>
+      <c r="D38" s="1">
         <v>5.2526841788116903</v>
       </c>
-      <c r="I38">
-        <f>D38+10</f>
+      <c r="E38" s="1">
         <v>16.52093004230122</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39" s="1">
         <v>44.346375781370398</v>
       </c>
-      <c r="B39">
+      <c r="C39" s="1">
         <v>37.937020380182901</v>
       </c>
-      <c r="C39">
-        <v>-6.6868487206836198</v>
-      </c>
-      <c r="D39">
-        <v>0.53592224216234297</v>
-      </c>
-      <c r="E39">
-        <v>37</v>
-      </c>
-      <c r="F39">
-        <f t="shared" si="0"/>
-        <v>44.346375781370398</v>
-      </c>
-      <c r="G39">
-        <f t="shared" si="4"/>
-        <v>37.937020380182901</v>
-      </c>
-      <c r="H39">
-        <f t="shared" si="8"/>
+      <c r="D39" s="1">
         <v>5.3131512793163802</v>
       </c>
-      <c r="I39">
-        <f>D39+35</f>
+      <c r="E39" s="1">
         <v>35.535922242162343</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40" s="1">
         <v>-8.8181670261519596</v>
       </c>
-      <c r="B40">
+      <c r="C40" s="1">
         <v>51.533737710953197</v>
       </c>
-      <c r="C40">
-        <v>-6.9181073933301596</v>
-      </c>
-      <c r="D40">
-        <v>3.8643178432888501</v>
-      </c>
-      <c r="E40">
-        <v>38</v>
-      </c>
-      <c r="F40">
-        <f t="shared" si="0"/>
-        <v>-8.8181670261519596</v>
-      </c>
-      <c r="G40">
-        <f t="shared" si="4"/>
-        <v>51.533737710953197</v>
-      </c>
-      <c r="H40">
-        <f t="shared" si="8"/>
+      <c r="D40" s="1">
         <v>5.0818926066698404</v>
       </c>
-      <c r="I40">
-        <f>D40+50</f>
+      <c r="E40" s="1">
         <v>53.864317843288852</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41" s="1">
         <v>22.8875640464307</v>
       </c>
-      <c r="B41">
+      <c r="C41" s="1">
         <v>38.886242436318803</v>
       </c>
-      <c r="C41">
-        <v>-6.5448780216419804</v>
-      </c>
-      <c r="D41">
-        <v>6.0777047922883103</v>
-      </c>
-      <c r="E41">
-        <v>39</v>
-      </c>
-      <c r="F41">
-        <f t="shared" si="0"/>
-        <v>22.8875640464307</v>
-      </c>
-      <c r="G41">
-        <f t="shared" si="4"/>
-        <v>38.886242436318803</v>
-      </c>
-      <c r="H41">
-        <f t="shared" si="8"/>
+      <c r="D41" s="1">
         <v>5.4551219783580196</v>
       </c>
-      <c r="I41">
-        <f t="shared" ref="I41:I44" si="9">D41+50</f>
+      <c r="E41" s="1">
         <v>56.077704792288309</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42" s="1">
         <v>58.643033172553402</v>
       </c>
-      <c r="B42">
+      <c r="C42" s="1">
         <v>45.189539611382799</v>
       </c>
-      <c r="C42">
-        <v>-6.8015636053553497</v>
-      </c>
-      <c r="D42">
-        <v>1.8426598676456001</v>
-      </c>
-      <c r="E42">
-        <v>40</v>
-      </c>
-      <c r="F42">
-        <f t="shared" si="0"/>
-        <v>58.643033172553402</v>
-      </c>
-      <c r="G42">
-        <f t="shared" si="4"/>
-        <v>45.189539611382799</v>
-      </c>
-      <c r="H42">
-        <f t="shared" si="8"/>
+      <c r="D42" s="1">
         <v>5.1984363946446503</v>
       </c>
-      <c r="I42">
-        <f>D42+80</f>
+      <c r="E42" s="1">
         <v>81.842659867645594</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43" s="1">
         <v>28.918616242157</v>
       </c>
-      <c r="B43">
+      <c r="C43" s="1">
         <v>47.750266999125003</v>
       </c>
-      <c r="C43">
-        <v>-6.2810433325526303</v>
-      </c>
-      <c r="D43">
-        <v>4.3599424613697204</v>
-      </c>
-      <c r="E43">
-        <v>41</v>
-      </c>
-      <c r="F43">
-        <f t="shared" si="0"/>
-        <v>28.918616242157</v>
-      </c>
-      <c r="G43">
-        <f t="shared" si="4"/>
-        <v>47.750266999125003</v>
-      </c>
-      <c r="H43">
-        <f t="shared" si="8"/>
+      <c r="D43" s="1">
         <v>5.7189566674473697</v>
       </c>
-      <c r="I43">
-        <f>D43+59</f>
+      <c r="E43" s="1">
         <v>63.35994246136972</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44" s="1">
         <v>43.104513921089399</v>
       </c>
-      <c r="B44">
+      <c r="C44" s="1">
         <v>8.8738075075004499</v>
       </c>
-      <c r="C44">
-        <v>-6.8324162565671598</v>
-      </c>
-      <c r="D44">
-        <v>0.78234509539099295</v>
-      </c>
-      <c r="E44">
-        <v>42</v>
-      </c>
-      <c r="F44">
-        <f t="shared" si="0"/>
-        <v>43.104513921089399</v>
-      </c>
-      <c r="G44">
-        <f t="shared" si="4"/>
-        <v>8.8738075075004499</v>
-      </c>
-      <c r="H44">
-        <f>SUM(C44,12.5)</f>
+      <c r="D44" s="1">
         <v>5.6675837434328402</v>
       </c>
-      <c r="I44">
-        <f>D44+5</f>
+      <c r="E44" s="1">
         <v>5.7823450953909932</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45" s="1">
         <v>47.283574746965002</v>
       </c>
-      <c r="B45">
+      <c r="C45" s="1">
         <v>74.933097206812405</v>
       </c>
-      <c r="C45">
-        <v>-6.9335675121265696</v>
-      </c>
-      <c r="D45">
-        <v>1.47682569770144</v>
-      </c>
-      <c r="E45">
-        <v>43</v>
-      </c>
-      <c r="F45">
-        <f t="shared" si="0"/>
-        <v>47.283574746965002</v>
-      </c>
-      <c r="G45">
-        <f t="shared" si="4"/>
-        <v>74.933097206812405</v>
-      </c>
-      <c r="H45">
-        <f t="shared" ref="H45:H52" si="10">SUM(C45,12.5)</f>
+      <c r="D45" s="1">
         <v>5.5664324878734304</v>
       </c>
-      <c r="I45">
-        <f t="shared" ref="I38:I60" si="11">D45+35</f>
+      <c r="E45" s="1">
         <v>36.476825697701443</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46" s="1">
         <v>21.577035693221099</v>
       </c>
-      <c r="B46">
+      <c r="C46" s="1">
         <v>18.619713832960802</v>
       </c>
-      <c r="C46">
-        <v>-5.8095979538375504</v>
-      </c>
-      <c r="D46">
-        <v>6.0716019651704203</v>
-      </c>
-      <c r="E46">
-        <v>44</v>
-      </c>
-      <c r="F46">
-        <f t="shared" si="0"/>
-        <v>21.577035693221099</v>
-      </c>
-      <c r="G46">
-        <f t="shared" si="4"/>
-        <v>18.619713832960802</v>
-      </c>
-      <c r="H46">
-        <f t="shared" si="10"/>
+      <c r="D46" s="1">
         <v>6.6904020461624496</v>
       </c>
-      <c r="I46">
-        <f>D46+37</f>
+      <c r="E46" s="1">
         <v>43.071601965170423</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47" s="1">
         <v>21.0838055690155</v>
       </c>
-      <c r="B47">
+      <c r="C47" s="1">
         <v>56.355226732009903</v>
       </c>
-      <c r="C47">
-        <v>-6.7592782166666101</v>
-      </c>
-      <c r="D47">
-        <v>9.9011119719222105</v>
-      </c>
-      <c r="E47">
-        <v>45</v>
-      </c>
-      <c r="F47">
-        <f t="shared" si="0"/>
-        <v>21.0838055690155</v>
-      </c>
-      <c r="G47">
-        <f t="shared" si="4"/>
-        <v>56.355226732009903</v>
-      </c>
-      <c r="H47">
-        <f t="shared" si="10"/>
+      <c r="D47" s="1">
         <v>5.7407217833333899</v>
       </c>
-      <c r="I47">
-        <f>D47+75</f>
+      <c r="E47" s="1">
         <v>84.901111971922205</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48" s="1">
         <v>40.860420278220502</v>
       </c>
-      <c r="B48">
+      <c r="C48" s="1">
         <v>29.1660102108312</v>
       </c>
-      <c r="C48">
-        <v>-6.4948567214412103</v>
-      </c>
-      <c r="D48">
-        <v>0.222443189780582</v>
-      </c>
-      <c r="E48">
-        <v>46</v>
-      </c>
-      <c r="F48">
-        <f t="shared" si="0"/>
-        <v>40.860420278220502</v>
-      </c>
-      <c r="G48">
-        <f t="shared" si="4"/>
-        <v>29.1660102108312</v>
-      </c>
-      <c r="H48">
-        <f t="shared" si="10"/>
+      <c r="D48" s="1">
         <v>6.0051432785587897</v>
       </c>
-      <c r="I48">
-        <f t="shared" si="11"/>
+      <c r="E48" s="1">
         <v>35.222443189780584</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49" s="1">
         <v>69.804490495749505</v>
       </c>
-      <c r="B49">
+      <c r="C49" s="1">
         <v>27.385931459651101</v>
       </c>
-      <c r="C49">
-        <v>-5.2465083452076797</v>
-      </c>
-      <c r="D49">
-        <v>0.69557459500384</v>
-      </c>
-      <c r="E49">
-        <v>47</v>
-      </c>
-      <c r="F49">
-        <f t="shared" si="0"/>
-        <v>69.804490495749505</v>
-      </c>
-      <c r="G49">
-        <f t="shared" si="4"/>
-        <v>27.385931459651101</v>
-      </c>
-      <c r="H49">
-        <f t="shared" si="10"/>
+      <c r="D49" s="1">
         <v>7.2534916547923203</v>
       </c>
-      <c r="I49">
-        <f>D49+94</f>
+      <c r="E49" s="1">
         <v>94.695574595003833</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50" s="1">
         <v>33.366444947843</v>
       </c>
-      <c r="B50">
+      <c r="C50" s="1">
         <v>23.2338358181388</v>
       </c>
-      <c r="C50">
-        <v>-5.9515390214645398</v>
-      </c>
-      <c r="D50">
-        <v>1.6949726365262501</v>
-      </c>
-      <c r="E50">
-        <v>48</v>
-      </c>
-      <c r="F50">
-        <f t="shared" si="0"/>
-        <v>33.366444947843</v>
-      </c>
-      <c r="G50">
-        <f t="shared" si="4"/>
-        <v>23.2338358181388</v>
-      </c>
-      <c r="H50">
-        <f t="shared" si="10"/>
+      <c r="D50" s="1">
         <v>6.5484609785354602</v>
       </c>
-      <c r="I50">
-        <f t="shared" si="11"/>
+      <c r="E50" s="1">
         <v>36.694972636526252</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51" s="1">
         <v>25.202712980637202</v>
       </c>
-      <c r="B51">
+      <c r="C51" s="1">
         <v>24.593086308373898</v>
       </c>
-      <c r="C51">
-        <v>-5.8982460902473601</v>
-      </c>
-      <c r="D51">
-        <v>1.67872746342801</v>
-      </c>
-      <c r="E51">
-        <v>49</v>
-      </c>
-      <c r="F51">
-        <f t="shared" si="0"/>
-        <v>25.202712980637202</v>
-      </c>
-      <c r="G51">
-        <f t="shared" si="4"/>
-        <v>24.593086308373898</v>
-      </c>
-      <c r="H51">
-        <f t="shared" si="10"/>
+      <c r="D51" s="1">
         <v>6.6017539097526399</v>
       </c>
-      <c r="I51">
-        <f>D51+75</f>
+      <c r="E51" s="1">
         <v>76.678727463428004</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52" s="1">
         <v>33.917428893140503</v>
       </c>
-      <c r="B52">
+      <c r="C52" s="1">
         <v>-1.63319148067065</v>
       </c>
-      <c r="C52">
-        <v>-6.8269276514287096</v>
-      </c>
-      <c r="D52">
-        <v>0.55019225000701999</v>
-      </c>
-      <c r="E52">
-        <v>50</v>
-      </c>
-      <c r="F52">
-        <f t="shared" si="0"/>
-        <v>33.917428893140503</v>
-      </c>
-      <c r="G52">
-        <f t="shared" si="4"/>
-        <v>-1.63319148067065</v>
-      </c>
-      <c r="H52">
-        <f t="shared" si="10"/>
+      <c r="D52" s="1">
         <v>5.6730723485712904</v>
       </c>
-      <c r="I52">
-        <f>D52+45</f>
+      <c r="E52" s="1">
         <v>45.550192250007022</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="B53" s="1">
         <v>31.689740329847801</v>
       </c>
-      <c r="B53">
+      <c r="C53" s="1">
         <v>36.6114803755965</v>
       </c>
-      <c r="C53">
-        <v>-6.8520763559115299</v>
-      </c>
-      <c r="D53">
-        <v>4.5845897348850997</v>
-      </c>
-      <c r="E53">
-        <v>51</v>
-      </c>
-      <c r="F53">
-        <f t="shared" si="0"/>
-        <v>31.689740329847801</v>
-      </c>
-      <c r="G53">
-        <f t="shared" si="4"/>
-        <v>36.6114803755965</v>
-      </c>
-      <c r="H53">
-        <f t="shared" si="1"/>
+      <c r="D53" s="1">
         <v>3.1479236440884701</v>
       </c>
-      <c r="I53">
-        <f>D53+55</f>
+      <c r="E53" s="1">
         <v>59.5845897348851</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54" s="1">
         <v>104.232395769535</v>
       </c>
-      <c r="B54">
+      <c r="C54" s="1">
         <v>25.699741100384099</v>
       </c>
-      <c r="C54">
-        <v>-6.88648024292206</v>
-      </c>
-      <c r="D54">
-        <v>0.46312421140527399</v>
-      </c>
-      <c r="E54">
-        <v>52</v>
-      </c>
-      <c r="F54">
-        <f t="shared" si="0"/>
-        <v>104.232395769535</v>
-      </c>
-      <c r="G54">
-        <f t="shared" si="4"/>
-        <v>25.699741100384099</v>
-      </c>
-      <c r="H54">
-        <f t="shared" si="1"/>
+      <c r="D54" s="1">
         <v>3.11351975707794</v>
       </c>
-      <c r="I54">
-        <f t="shared" ref="I54:I56" si="12">D54+55</f>
+      <c r="E54" s="1">
         <v>55.463124211405272</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="1">
+        <v>53</v>
+      </c>
+      <c r="B55" s="1">
         <v>54.615890605128598</v>
       </c>
-      <c r="B55">
+      <c r="C55" s="1">
         <v>26.6644155662316</v>
       </c>
-      <c r="C55">
-        <v>-5.8985507265265502</v>
-      </c>
-      <c r="D55">
-        <v>6.6272727859873903</v>
-      </c>
-      <c r="E55">
-        <v>53</v>
-      </c>
-      <c r="F55">
-        <f t="shared" si="0"/>
-        <v>54.615890605128598</v>
-      </c>
-      <c r="G55">
-        <f t="shared" si="4"/>
-        <v>26.6644155662316</v>
-      </c>
-      <c r="H55">
-        <f t="shared" si="1"/>
+      <c r="D55" s="1">
         <v>4.1014492734734498</v>
       </c>
-      <c r="I55">
-        <f t="shared" si="12"/>
+      <c r="E55" s="1">
         <v>61.627272785987387</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="B56" s="1">
         <v>141.12474963266999</v>
       </c>
-      <c r="B56">
+      <c r="C56" s="1">
         <v>22.100067369981002</v>
       </c>
-      <c r="C56">
-        <v>-5.8925079479051297</v>
-      </c>
-      <c r="D56">
-        <v>1.0299070000675301</v>
-      </c>
-      <c r="E56">
-        <v>54</v>
-      </c>
-      <c r="F56">
-        <f t="shared" si="0"/>
-        <v>141.12474963266999</v>
-      </c>
-      <c r="G56">
-        <f t="shared" si="4"/>
-        <v>22.100067369981002</v>
-      </c>
-      <c r="H56">
-        <f t="shared" si="1"/>
+      <c r="D56" s="1">
         <v>4.1074920520948703</v>
       </c>
-      <c r="I56">
-        <f t="shared" si="12"/>
+      <c r="E56" s="1">
         <v>56.029907000067531</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57" s="1">
         <v>68.464837437905302</v>
       </c>
-      <c r="B57">
+      <c r="C57" s="1">
         <v>55.9670321805228</v>
       </c>
-      <c r="C57">
-        <v>-5.4839264523528302</v>
-      </c>
-      <c r="D57">
-        <v>1.25011854725561</v>
-      </c>
-      <c r="E57">
-        <v>55</v>
-      </c>
-      <c r="F57">
-        <f t="shared" si="0"/>
-        <v>68.464837437905302</v>
-      </c>
-      <c r="G57">
-        <f t="shared" si="4"/>
-        <v>55.9670321805228</v>
-      </c>
-      <c r="H57">
-        <f>SUM(C57,13)</f>
+      <c r="D57" s="1">
         <v>7.5160735476471698</v>
       </c>
-      <c r="I57">
-        <f>D57+60</f>
+      <c r="E57" s="1">
         <v>61.25011854725561</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="B58" s="1">
         <v>59.630690059532299</v>
       </c>
-      <c r="B58">
+      <c r="C58" s="1">
         <v>71.530547202223701</v>
       </c>
-      <c r="C58">
-        <v>-6.7052851275313898</v>
-      </c>
-      <c r="D58">
-        <v>0.86905021213501898</v>
-      </c>
-      <c r="E58">
-        <v>56</v>
-      </c>
-      <c r="F58">
-        <f t="shared" si="0"/>
-        <v>59.630690059532299</v>
-      </c>
-      <c r="G58">
-        <f t="shared" si="4"/>
-        <v>71.530547202223701</v>
-      </c>
-      <c r="H58">
-        <f t="shared" ref="H58:H75" si="13">SUM(C58,13)</f>
+      <c r="D58" s="1">
         <v>6.2947148724686102</v>
       </c>
-      <c r="I58">
-        <f t="shared" si="11"/>
+      <c r="E58" s="1">
         <v>35.869050212135022</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="1">
+        <v>57</v>
+      </c>
+      <c r="B59" s="1">
         <v>74.759387166159001</v>
       </c>
-      <c r="B59">
+      <c r="C59" s="1">
         <v>21.053171898819201</v>
       </c>
-      <c r="C59">
-        <v>-5.2414731071833902</v>
-      </c>
-      <c r="D59">
-        <v>9.2181304807095099</v>
-      </c>
-      <c r="E59">
-        <v>57</v>
-      </c>
-      <c r="F59">
-        <f t="shared" si="0"/>
-        <v>74.759387166159001</v>
-      </c>
-      <c r="G59">
-        <f t="shared" si="4"/>
-        <v>21.053171898819201</v>
-      </c>
-      <c r="H59">
-        <f t="shared" si="13"/>
+      <c r="D59" s="1">
         <v>7.7585268928166098</v>
       </c>
-      <c r="I59">
-        <f t="shared" si="11"/>
+      <c r="E59" s="1">
         <v>44.218130480709512</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="1">
+        <v>58</v>
+      </c>
+      <c r="B60" s="1">
         <v>132.67130492549001</v>
       </c>
-      <c r="B60">
+      <c r="C60" s="1">
         <v>16.525706047040501</v>
       </c>
-      <c r="C60">
-        <v>-6.9458191107593699</v>
-      </c>
-      <c r="D60">
-        <v>0.27368156550394201</v>
-      </c>
-      <c r="E60">
-        <v>58</v>
-      </c>
-      <c r="F60">
-        <f t="shared" si="0"/>
-        <v>132.67130492549001</v>
-      </c>
-      <c r="G60">
-        <f t="shared" si="4"/>
-        <v>16.525706047040501</v>
-      </c>
-      <c r="H60">
-        <f t="shared" si="13"/>
+      <c r="D60" s="1">
         <v>6.0541808892406301</v>
       </c>
-      <c r="I60">
-        <f>D60+98</f>
+      <c r="E60" s="1">
         <v>98.273681565503935</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="1">
+        <v>59</v>
+      </c>
+      <c r="B61" s="1">
         <v>28.846923199464001</v>
       </c>
-      <c r="B61">
+      <c r="C61" s="1">
         <v>110.017294069991</v>
       </c>
-      <c r="C61">
-        <v>-6.9163392897795601</v>
-      </c>
-      <c r="D61">
-        <v>4.8743736447380703</v>
-      </c>
-      <c r="E61">
-        <v>59</v>
-      </c>
-      <c r="F61">
-        <f t="shared" si="0"/>
-        <v>28.846923199464001</v>
-      </c>
-      <c r="G61">
-        <f t="shared" si="4"/>
-        <v>110.017294069991</v>
-      </c>
-      <c r="H61">
-        <f t="shared" si="13"/>
+      <c r="D61" s="1">
         <v>6.0836607102204399</v>
       </c>
-      <c r="I61">
-        <f>D61+54</f>
+      <c r="E61" s="1">
         <v>58.874373644738071</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="1">
+        <v>60</v>
+      </c>
+      <c r="B62" s="1">
         <v>79.561446783541101</v>
       </c>
-      <c r="B62">
+      <c r="C62" s="1">
         <v>53.8205221251336</v>
       </c>
-      <c r="C62">
-        <v>-5.8910839277833302</v>
-      </c>
-      <c r="D62">
-        <v>4.4846901788194602</v>
-      </c>
-      <c r="E62">
-        <v>60</v>
-      </c>
-      <c r="F62">
-        <f t="shared" si="0"/>
-        <v>79.561446783541101</v>
-      </c>
-      <c r="G62">
-        <f t="shared" si="4"/>
-        <v>53.8205221251336</v>
-      </c>
-      <c r="H62">
-        <f t="shared" si="13"/>
+      <c r="D62" s="1">
         <v>7.1089160722166698</v>
       </c>
-      <c r="I62">
-        <f>D62+80</f>
+      <c r="E62" s="1">
         <v>84.484690178819463</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="1">
+        <v>61</v>
+      </c>
+      <c r="B63" s="1">
         <v>55.887978012679199</v>
       </c>
-      <c r="B63">
+      <c r="C63" s="1">
         <v>46.436992722736498</v>
       </c>
-      <c r="C63">
-        <v>-6.3094908985218101</v>
-      </c>
-      <c r="D63">
-        <v>6.2267054912016704</v>
-      </c>
-      <c r="E63">
-        <v>61</v>
-      </c>
-      <c r="F63">
-        <f t="shared" si="0"/>
-        <v>55.887978012679199</v>
-      </c>
-      <c r="G63">
-        <f t="shared" si="4"/>
-        <v>46.436992722736498</v>
-      </c>
-      <c r="H63">
-        <f t="shared" si="13"/>
+      <c r="D63" s="1">
         <v>6.6905091014781899</v>
       </c>
-      <c r="I63">
-        <f>D63+61</f>
+      <c r="E63" s="1">
         <v>67.22670549120167</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" s="1">
+        <v>62</v>
+      </c>
+      <c r="B64" s="1">
         <v>42.571241845267799</v>
       </c>
-      <c r="B64">
+      <c r="C64" s="1">
         <v>28.5609472920274</v>
       </c>
-      <c r="C64">
-        <v>-7.0199824805258002</v>
-      </c>
-      <c r="D64">
-        <v>0.594844461884253</v>
-      </c>
-      <c r="E64">
-        <v>62</v>
-      </c>
-      <c r="F64">
-        <f t="shared" si="0"/>
-        <v>42.571241845267799</v>
-      </c>
-      <c r="G64">
-        <f t="shared" si="4"/>
-        <v>28.5609472920274</v>
-      </c>
-      <c r="H64">
-        <f t="shared" si="13"/>
+      <c r="D64" s="1">
         <v>5.9800175194741998</v>
       </c>
-      <c r="I64">
-        <f>D64+78</f>
+      <c r="E64" s="1">
         <v>78.59484446188425</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="1">
+        <v>63</v>
+      </c>
+      <c r="B65" s="1">
         <v>48.780289055571899</v>
       </c>
-      <c r="B65">
+      <c r="C65" s="1">
         <v>-20.596552162590701</v>
       </c>
-      <c r="C65">
-        <v>-6.95543499381382</v>
-      </c>
-      <c r="D65">
-        <v>6.2377851018758603</v>
-      </c>
-      <c r="E65">
-        <v>63</v>
-      </c>
-      <c r="F65">
-        <f t="shared" si="0"/>
-        <v>48.780289055571899</v>
-      </c>
-      <c r="G65">
-        <f t="shared" si="4"/>
-        <v>-20.596552162590701</v>
-      </c>
-      <c r="H65">
-        <f t="shared" si="13"/>
+      <c r="D65" s="1">
         <v>6.04456500618618</v>
       </c>
-      <c r="I65">
-        <f>D65+39</f>
+      <c r="E65" s="1">
         <v>45.237785101875858</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="1">
+        <v>64</v>
+      </c>
+      <c r="B66" s="1">
         <v>42.104894778808799</v>
       </c>
-      <c r="B66">
+      <c r="C66" s="1">
         <v>22.473711916916301</v>
       </c>
-      <c r="C66">
-        <v>-6.9246760768896598</v>
-      </c>
-      <c r="D66">
-        <v>0.192259740746545</v>
-      </c>
-      <c r="E66">
-        <v>64</v>
-      </c>
-      <c r="F66">
-        <f t="shared" si="0"/>
-        <v>42.104894778808799</v>
-      </c>
-      <c r="G66">
-        <f t="shared" si="4"/>
-        <v>22.473711916916301</v>
-      </c>
-      <c r="H66">
-        <f t="shared" si="13"/>
+      <c r="D66" s="1">
         <v>6.0753239231103402</v>
       </c>
-      <c r="I66">
-        <f t="shared" ref="I63:I67" si="14">D66+39</f>
+      <c r="E66" s="1">
         <v>39.192259740746543</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="1">
+        <v>65</v>
+      </c>
+      <c r="B67" s="1">
         <v>56.362942806705</v>
       </c>
-      <c r="B67">
+      <c r="C67" s="1">
         <v>37.953417550894002</v>
       </c>
-      <c r="C67">
-        <v>-5.9015285546489702</v>
-      </c>
-      <c r="D67">
-        <v>6.7771582327370501</v>
-      </c>
-      <c r="E67">
-        <v>65</v>
-      </c>
-      <c r="F67">
-        <f t="shared" ref="F67:F101" si="15">A67</f>
-        <v>56.362942806705</v>
-      </c>
-      <c r="G67">
-        <f t="shared" ref="G67:G101" si="16">B67</f>
-        <v>37.953417550894002</v>
-      </c>
-      <c r="H67">
-        <f t="shared" si="13"/>
+      <c r="D67" s="1">
         <v>7.0984714453510298</v>
       </c>
-      <c r="I67">
-        <f>D67+90</f>
+      <c r="E67" s="1">
         <v>96.777158232737051</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="1">
+        <v>66</v>
+      </c>
+      <c r="B68" s="1">
         <v>44.717949113242703</v>
       </c>
-      <c r="B68">
+      <c r="C68" s="1">
         <v>32.982050233552698</v>
       </c>
-      <c r="C68">
-        <v>-5.9724119328111396</v>
-      </c>
-      <c r="D68">
-        <v>6.2491737303960404</v>
-      </c>
-      <c r="E68">
-        <v>66</v>
-      </c>
-      <c r="F68">
-        <f t="shared" si="15"/>
-        <v>44.717949113242703</v>
-      </c>
-      <c r="G68">
-        <f t="shared" si="16"/>
-        <v>32.982050233552698</v>
-      </c>
-      <c r="H68">
-        <f t="shared" si="13"/>
+      <c r="D68" s="1">
         <v>7.0275880671888604</v>
       </c>
-      <c r="I68">
-        <f>D68+75</f>
+      <c r="E68" s="1">
         <v>81.249173730396038</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A69">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" s="1">
+        <v>67</v>
+      </c>
+      <c r="B69" s="1">
         <v>57.868981162068501</v>
       </c>
-      <c r="B69">
+      <c r="C69" s="1">
         <v>20.466728005495799</v>
       </c>
-      <c r="C69">
-        <v>-6.9074313362038904</v>
-      </c>
-      <c r="D69">
-        <v>7.74890393882675</v>
-      </c>
-      <c r="E69">
-        <v>67</v>
-      </c>
-      <c r="F69">
-        <f t="shared" si="15"/>
-        <v>57.868981162068501</v>
-      </c>
-      <c r="G69">
-        <f t="shared" si="16"/>
-        <v>20.466728005495799</v>
-      </c>
-      <c r="H69">
-        <f t="shared" si="13"/>
+      <c r="D69" s="1">
         <v>6.0925686637961096</v>
       </c>
-      <c r="I69">
-        <f t="shared" ref="I69:I70" si="17">D69+75</f>
+      <c r="E69" s="1">
         <v>82.748903938826743</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A70">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="1">
+        <v>68</v>
+      </c>
+      <c r="B70" s="1">
         <v>70.996094701358004</v>
       </c>
-      <c r="B70">
+      <c r="C70" s="1">
         <v>25.166195867842902</v>
       </c>
-      <c r="C70">
-        <v>-5.2952763785159496</v>
-      </c>
-      <c r="D70">
-        <v>2.34466263883145</v>
-      </c>
-      <c r="E70">
-        <v>68</v>
-      </c>
-      <c r="F70">
-        <f t="shared" si="15"/>
-        <v>70.996094701358004</v>
-      </c>
-      <c r="G70">
-        <f t="shared" si="16"/>
-        <v>25.166195867842902</v>
-      </c>
-      <c r="H70">
-        <f t="shared" si="13"/>
+      <c r="D70" s="1">
         <v>7.7047236214840504</v>
       </c>
-      <c r="I70">
-        <f t="shared" si="17"/>
+      <c r="E70" s="1">
         <v>77.344662638831451</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A71">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="1">
+        <v>69</v>
+      </c>
+      <c r="B71" s="1">
         <v>51.097029582573498</v>
       </c>
-      <c r="B71">
+      <c r="C71" s="1">
         <v>-60.914582886871599</v>
       </c>
-      <c r="C71">
-        <v>-6.9120923553720504</v>
-      </c>
-      <c r="D71">
-        <v>6.12889448581201</v>
-      </c>
-      <c r="E71">
-        <v>69</v>
-      </c>
-      <c r="F71">
-        <f t="shared" si="15"/>
-        <v>51.097029582573498</v>
-      </c>
-      <c r="G71">
-        <f t="shared" si="16"/>
-        <v>-60.914582886871599</v>
-      </c>
-      <c r="H71">
-        <f t="shared" si="13"/>
+      <c r="D71" s="1">
         <v>6.0879076446279496</v>
       </c>
-      <c r="I71">
-        <f>D71+4</f>
+      <c r="E71" s="1">
         <v>10.12889448581201</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A72">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" s="1">
+        <v>70</v>
+      </c>
+      <c r="B72" s="1">
         <v>43.061600518754702</v>
       </c>
-      <c r="B72">
+      <c r="C72" s="1">
         <v>15.292745444072899</v>
       </c>
-      <c r="C72">
-        <v>-5.9232545740444502</v>
-      </c>
-      <c r="D72">
-        <v>0.191891172730079</v>
-      </c>
-      <c r="E72">
-        <v>70</v>
-      </c>
-      <c r="F72">
-        <f t="shared" si="15"/>
-        <v>43.061600518754702</v>
-      </c>
-      <c r="G72">
-        <f t="shared" si="16"/>
-        <v>15.292745444072899</v>
-      </c>
-      <c r="H72">
-        <f t="shared" si="13"/>
+      <c r="D72" s="1">
         <v>7.0767454259555498</v>
       </c>
-      <c r="I72">
-        <f>D72+86</f>
+      <c r="E72" s="1">
         <v>86.191891172730081</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A73">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" s="1">
+        <v>71</v>
+      </c>
+      <c r="B73" s="1">
         <v>50.511159650379497</v>
       </c>
-      <c r="B73">
+      <c r="C73" s="1">
         <v>27.8823699576932</v>
       </c>
-      <c r="C73">
-        <v>-6.0357675519007596</v>
-      </c>
-      <c r="D73">
-        <v>4.9121061404623996</v>
-      </c>
-      <c r="E73">
-        <v>71</v>
-      </c>
-      <c r="F73">
-        <f t="shared" si="15"/>
-        <v>50.511159650379497</v>
-      </c>
-      <c r="G73">
-        <f t="shared" si="16"/>
-        <v>27.8823699576932</v>
-      </c>
-      <c r="H73">
-        <f t="shared" si="13"/>
+      <c r="D73" s="1">
         <v>6.9642324480992404</v>
       </c>
-      <c r="I73">
-        <f>D73+86</f>
+      <c r="E73" s="1">
         <v>90.912106140462399</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A74">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" s="1">
+        <v>72</v>
+      </c>
+      <c r="B74" s="1">
         <v>58.894293825507901</v>
       </c>
-      <c r="B74">
+      <c r="C74" s="1">
         <v>19.6876245419428</v>
       </c>
-      <c r="C74">
-        <v>-5.74519666796665</v>
-      </c>
-      <c r="D74">
-        <v>0.98522681175388804</v>
-      </c>
-      <c r="E74">
-        <v>72</v>
-      </c>
-      <c r="F74">
-        <f t="shared" si="15"/>
-        <v>58.894293825507901</v>
-      </c>
-      <c r="G74">
-        <f t="shared" si="16"/>
-        <v>19.6876245419428</v>
-      </c>
-      <c r="H74">
-        <f t="shared" si="13"/>
+      <c r="D74" s="1">
         <v>7.25480333203335</v>
       </c>
-      <c r="I74">
-        <f>D74+78</f>
+      <c r="E74" s="1">
         <v>78.98522681175389</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A75">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" s="1">
+        <v>73</v>
+      </c>
+      <c r="B75" s="1">
         <v>49.164186654985897</v>
       </c>
-      <c r="B75">
+      <c r="C75" s="1">
         <v>80.790504727367704</v>
       </c>
-      <c r="C75">
-        <v>-6.2659921602033899</v>
-      </c>
-      <c r="D75">
-        <v>2.9463687738581501</v>
-      </c>
-      <c r="E75">
-        <v>73</v>
-      </c>
-      <c r="F75">
-        <f t="shared" si="15"/>
-        <v>49.164186654985897</v>
-      </c>
-      <c r="G75">
-        <f t="shared" si="16"/>
-        <v>80.790504727367704</v>
-      </c>
-      <c r="H75">
-        <f t="shared" si="13"/>
+      <c r="D75" s="1">
         <v>6.7340078397966101</v>
       </c>
-      <c r="I75">
-        <f t="shared" ref="I73:I78" si="18">D75+62</f>
+      <c r="E75" s="1">
         <v>64.946368773858154</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A76">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" s="1">
+        <v>74</v>
+      </c>
+      <c r="B76" s="1">
         <v>54.2000083957032</v>
       </c>
-      <c r="B76">
+      <c r="C76" s="1">
         <v>82.535213896541606</v>
       </c>
-      <c r="C76">
-        <v>-6.28345275862719</v>
-      </c>
-      <c r="D76">
-        <v>6.31809358238384</v>
-      </c>
-      <c r="E76">
-        <v>74</v>
-      </c>
-      <c r="F76">
-        <f t="shared" si="15"/>
-        <v>54.2000083957032</v>
-      </c>
-      <c r="G76">
-        <f t="shared" si="16"/>
-        <v>82.535213896541606</v>
-      </c>
-      <c r="H76">
-        <f>SUM(C76,10)</f>
+      <c r="D76" s="1">
         <v>3.71654724137281</v>
       </c>
-      <c r="I76">
-        <f>D76+83</f>
+      <c r="E76" s="1">
         <v>89.318093582383838</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A77">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" s="1">
+        <v>75</v>
+      </c>
+      <c r="B77" s="1">
         <v>54.4807773748988</v>
       </c>
-      <c r="B77">
+      <c r="C77" s="1">
         <v>4.6235080679257203</v>
       </c>
-      <c r="C77">
-        <v>-6.1502982148625804</v>
-      </c>
-      <c r="D77">
-        <v>1.8426742012517401</v>
-      </c>
-      <c r="E77">
-        <v>75</v>
-      </c>
-      <c r="F77">
-        <f t="shared" si="15"/>
-        <v>54.4807773748988</v>
-      </c>
-      <c r="G77">
-        <f t="shared" si="16"/>
-        <v>4.6235080679257203</v>
-      </c>
-      <c r="H77">
-        <f>SUM(C77,12.5)</f>
+      <c r="D77" s="1">
         <v>6.3497017851374196</v>
       </c>
-      <c r="I77">
-        <f>D77+76</f>
+      <c r="E77" s="1">
         <v>77.842674201251739</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A78">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78" s="1">
+        <v>76</v>
+      </c>
+      <c r="B78" s="1">
         <v>75.328529763607904</v>
       </c>
-      <c r="B78">
+      <c r="C78" s="1">
         <v>48.252803567418802</v>
       </c>
-      <c r="C78">
-        <v>-5.3842747728327698</v>
-      </c>
-      <c r="D78">
-        <v>-0.32580492279186701</v>
-      </c>
-      <c r="E78">
-        <v>76</v>
-      </c>
-      <c r="F78">
-        <f t="shared" si="15"/>
-        <v>75.328529763607904</v>
-      </c>
-      <c r="G78">
-        <f t="shared" si="16"/>
-        <v>48.252803567418802</v>
-      </c>
-      <c r="H78">
-        <f t="shared" ref="H78:H86" si="19">SUM(C78,12.5)</f>
+      <c r="D78" s="1">
         <v>7.1157252271672302</v>
       </c>
-      <c r="I78">
-        <f>D78+103</f>
+      <c r="E78" s="1">
         <v>102.67419507720814</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79" s="1">
+        <v>77</v>
+      </c>
+      <c r="B79" s="1">
         <v>57.052085635734798</v>
       </c>
-      <c r="B79">
+      <c r="C79" s="1">
         <v>-10.9543369915199</v>
       </c>
-      <c r="C79">
-        <v>-5.7584493947964699</v>
-      </c>
-      <c r="D79">
-        <v>0.174705221286866</v>
-      </c>
-      <c r="E79">
-        <v>77</v>
-      </c>
-      <c r="F79">
-        <f t="shared" si="15"/>
-        <v>57.052085635734798</v>
-      </c>
-      <c r="G79">
-        <f t="shared" si="16"/>
-        <v>-10.9543369915199</v>
-      </c>
-      <c r="H79">
-        <f t="shared" si="19"/>
+      <c r="D79" s="1">
         <v>6.7415506052035301</v>
       </c>
-      <c r="I79">
-        <f>D79+42</f>
+      <c r="E79" s="1">
         <v>42.174705221286864</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A80">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80" s="1">
+        <v>78</v>
+      </c>
+      <c r="B80" s="1">
         <v>55.051920285957301</v>
       </c>
-      <c r="B80">
+      <c r="C80" s="1">
         <v>4.5054433665970004</v>
       </c>
-      <c r="C80">
-        <v>-5.9644865186757201</v>
-      </c>
-      <c r="D80">
-        <v>3.89265075899685</v>
-      </c>
-      <c r="E80">
-        <v>78</v>
-      </c>
-      <c r="F80">
-        <f t="shared" si="15"/>
-        <v>55.051920285957301</v>
-      </c>
-      <c r="G80">
-        <f t="shared" si="16"/>
-        <v>4.5054433665970004</v>
-      </c>
-      <c r="H80">
-        <f t="shared" si="19"/>
+      <c r="D80" s="1">
         <v>6.5355134813242799</v>
       </c>
-      <c r="I80">
-        <f>D80+45</f>
+      <c r="E80" s="1">
         <v>48.892650758996851</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A81">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" s="1">
+        <v>79</v>
+      </c>
+      <c r="B81" s="1">
         <v>54.4874882597923</v>
       </c>
-      <c r="B81">
+      <c r="C81" s="1">
         <v>36.278635644830601</v>
       </c>
-      <c r="C81">
-        <v>-5.2749676788505697</v>
-      </c>
-      <c r="D81">
-        <v>0.54924348452605598</v>
-      </c>
-      <c r="E81">
-        <v>79</v>
-      </c>
-      <c r="F81">
-        <f t="shared" si="15"/>
-        <v>54.4874882597923</v>
-      </c>
-      <c r="G81">
-        <f t="shared" si="16"/>
-        <v>36.278635644830601</v>
-      </c>
-      <c r="H81">
-        <f t="shared" si="19"/>
+      <c r="D81" s="1">
         <v>7.2250323211494303</v>
       </c>
-      <c r="I81">
-        <f>D81+20</f>
+      <c r="E81" s="1">
         <v>20.549243484526055</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A82">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82" s="1">
+        <v>80</v>
+      </c>
+      <c r="B82" s="1">
         <v>51.764207213161903</v>
       </c>
-      <c r="B82">
+      <c r="C82" s="1">
         <v>44.709396660307704</v>
       </c>
-      <c r="C82">
-        <v>-5.7957005115587501</v>
-      </c>
-      <c r="D82">
-        <v>4.6996003541373899</v>
-      </c>
-      <c r="E82">
-        <v>80</v>
-      </c>
-      <c r="F82">
-        <f t="shared" si="15"/>
-        <v>51.764207213161903</v>
-      </c>
-      <c r="G82">
-        <f t="shared" si="16"/>
-        <v>44.709396660307704</v>
-      </c>
-      <c r="H82">
-        <f t="shared" si="19"/>
+      <c r="D82" s="1">
         <v>6.7042994884412499</v>
       </c>
-      <c r="I82">
-        <f>D82+123</f>
+      <c r="E82" s="1">
         <v>127.69960035413739</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A83">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83" s="1">
+        <v>81</v>
+      </c>
+      <c r="B83" s="1">
         <v>90.326892155079193</v>
       </c>
-      <c r="B83">
+      <c r="C83" s="1">
         <v>33.917106006707598</v>
       </c>
-      <c r="C83">
-        <v>-6.9306529255221996</v>
-      </c>
-      <c r="D83">
-        <v>5.4457865041930198</v>
-      </c>
-      <c r="E83">
-        <v>81</v>
-      </c>
-      <c r="F83">
-        <f t="shared" si="15"/>
-        <v>90.326892155079193</v>
-      </c>
-      <c r="G83">
-        <f t="shared" si="16"/>
-        <v>33.917106006707598</v>
-      </c>
-      <c r="H83">
-        <f t="shared" si="19"/>
+      <c r="D83" s="1">
         <v>5.5693470744778004</v>
       </c>
-      <c r="I83">
-        <f>D83+85</f>
+      <c r="E83" s="1">
         <v>90.445786504193023</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84" s="1">
+        <v>82</v>
+      </c>
+      <c r="B84" s="1">
         <v>38.619155301725201</v>
       </c>
-      <c r="B84">
+      <c r="C84" s="1">
         <v>3.8592449200672698</v>
       </c>
-      <c r="C84">
-        <v>-7.5770211146599298</v>
-      </c>
-      <c r="D84">
-        <v>8.7713341361559305</v>
-      </c>
-      <c r="E84">
-        <v>82</v>
-      </c>
-      <c r="F84">
-        <f t="shared" si="15"/>
-        <v>38.619155301725201</v>
-      </c>
-      <c r="G84">
-        <f t="shared" si="16"/>
-        <v>3.8592449200672698</v>
-      </c>
-      <c r="H84">
-        <f t="shared" si="19"/>
+      <c r="D84" s="1">
         <v>4.9229788853400702</v>
       </c>
-      <c r="I84">
-        <f t="shared" ref="I84:I87" si="20">D84+85</f>
+      <c r="E84" s="1">
         <v>93.771334136155929</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85" s="1">
+        <v>83</v>
+      </c>
+      <c r="B85" s="1">
         <v>54.724837369249499</v>
       </c>
-      <c r="B85">
+      <c r="C85" s="1">
         <v>33.246227686734201</v>
       </c>
-      <c r="C85">
-        <v>-6.9089847114649601</v>
-      </c>
-      <c r="D85">
-        <v>1.9213939203062</v>
-      </c>
-      <c r="E85">
-        <v>83</v>
-      </c>
-      <c r="F85">
-        <f t="shared" si="15"/>
-        <v>54.724837369249499</v>
-      </c>
-      <c r="G85">
-        <f t="shared" si="16"/>
-        <v>33.246227686734201</v>
-      </c>
-      <c r="H85">
-        <f t="shared" si="19"/>
+      <c r="D85" s="1">
         <v>5.5910152885350399</v>
       </c>
-      <c r="I85">
-        <f t="shared" si="20"/>
+      <c r="E85" s="1">
         <v>86.921393920306201</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A86">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86" s="1">
+        <v>84</v>
+      </c>
+      <c r="B86" s="1">
         <v>51.413965844639698</v>
       </c>
-      <c r="B86">
+      <c r="C86" s="1">
         <v>63.427592879123999</v>
       </c>
-      <c r="C86">
-        <v>-5.6562715008428999</v>
-      </c>
-      <c r="D86">
-        <v>10.210668182964801</v>
-      </c>
-      <c r="E86">
-        <v>84</v>
-      </c>
-      <c r="F86">
-        <f t="shared" si="15"/>
-        <v>51.413965844639698</v>
-      </c>
-      <c r="G86">
-        <f t="shared" si="16"/>
-        <v>63.427592879123999</v>
-      </c>
-      <c r="H86">
-        <f t="shared" si="19"/>
+      <c r="D86" s="1">
         <v>6.8437284991571001</v>
       </c>
-      <c r="I86">
-        <f>D86+95</f>
+      <c r="E86" s="1">
         <v>105.2106681829648</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A87">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87" s="1">
+        <v>85</v>
+      </c>
+      <c r="B87" s="1">
         <v>64.396320408290194</v>
       </c>
-      <c r="B87">
+      <c r="C87" s="1">
         <v>34.826096560841201</v>
       </c>
-      <c r="C87">
-        <v>-5.8518525971316704</v>
-      </c>
-      <c r="D87">
-        <v>5.3039078814675502</v>
-      </c>
-      <c r="E87">
-        <v>85</v>
-      </c>
-      <c r="F87">
-        <f t="shared" si="15"/>
-        <v>64.396320408290194</v>
-      </c>
-      <c r="G87">
-        <f t="shared" si="16"/>
-        <v>34.826096560841201</v>
-      </c>
-      <c r="H87">
-        <f t="shared" ref="H67:H101" si="21">SUM(C87,10)</f>
+      <c r="D87" s="1">
         <v>4.1481474028683296</v>
       </c>
-      <c r="I87">
-        <f>D87+85</f>
+      <c r="E87" s="1">
         <v>90.303907881467552</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A88">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" s="1">
+        <v>86</v>
+      </c>
+      <c r="B88" s="1">
         <v>47.599158300902701</v>
       </c>
-      <c r="B88">
+      <c r="C88" s="1">
         <v>35.604212320198897</v>
       </c>
-      <c r="C88">
-        <v>-6.35665568582424</v>
-      </c>
-      <c r="D88">
-        <v>0.71582250090338895</v>
-      </c>
-      <c r="E88">
-        <v>86</v>
-      </c>
-      <c r="F88">
-        <f t="shared" si="15"/>
-        <v>47.599158300902701</v>
-      </c>
-      <c r="G88">
-        <f t="shared" si="16"/>
-        <v>35.604212320198897</v>
-      </c>
-      <c r="H88">
-        <f>SUM(C88,13.5)</f>
+      <c r="D88" s="1">
         <v>7.14334431417576</v>
       </c>
-      <c r="I88">
-        <f t="shared" ref="I88:I89" si="22">D88+78</f>
+      <c r="E88" s="1">
         <v>78.715822500903386</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A89">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89" s="1">
+        <v>87</v>
+      </c>
+      <c r="B89" s="1">
         <v>51.887765258755998</v>
       </c>
-      <c r="B89">
+      <c r="C89" s="1">
         <v>38.715701363419697</v>
       </c>
-      <c r="C89">
-        <v>-6.9115590680177599</v>
-      </c>
-      <c r="D89">
-        <v>1.2887501054302899</v>
-      </c>
-      <c r="E89">
-        <v>87</v>
-      </c>
-      <c r="F89">
-        <f t="shared" si="15"/>
-        <v>51.887765258755998</v>
-      </c>
-      <c r="G89">
-        <f t="shared" si="16"/>
-        <v>38.715701363419697</v>
-      </c>
-      <c r="H89">
-        <f t="shared" ref="H89:H94" si="23">SUM(C89,13.5)</f>
+      <c r="D89" s="1">
         <v>6.5884409319822401</v>
       </c>
-      <c r="I89">
-        <f>D89+83</f>
+      <c r="E89" s="1">
         <v>84.288750105430296</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A90">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90" s="1">
+        <v>88</v>
+      </c>
+      <c r="B90" s="1">
         <v>55.940788301009498</v>
       </c>
-      <c r="B90">
+      <c r="C90" s="1">
         <v>29.694013935080601</v>
       </c>
-      <c r="C90">
-        <v>-5.8960244759313003</v>
-      </c>
-      <c r="D90">
-        <v>8.2160745782863192</v>
-      </c>
-      <c r="E90">
-        <v>88</v>
-      </c>
-      <c r="F90">
-        <f t="shared" si="15"/>
-        <v>55.940788301009498</v>
-      </c>
-      <c r="G90">
-        <f t="shared" si="16"/>
-        <v>29.694013935080601</v>
-      </c>
-      <c r="H90">
-        <f t="shared" si="23"/>
+      <c r="D90" s="1">
         <v>7.6039755240686997</v>
       </c>
-      <c r="I90">
-        <f>D90+26</f>
+      <c r="E90" s="1">
         <v>34.216074578286317</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A91">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91" s="1">
+        <v>89</v>
+      </c>
+      <c r="B91" s="1">
         <v>72.412429295758798</v>
       </c>
-      <c r="B91">
+      <c r="C91" s="1">
         <v>24.7899257033536</v>
       </c>
-      <c r="C91">
-        <v>-5.8627357377238098</v>
-      </c>
-      <c r="D91">
-        <v>7.5008946176279503</v>
-      </c>
-      <c r="E91">
-        <v>89</v>
-      </c>
-      <c r="F91">
-        <f t="shared" si="15"/>
-        <v>72.412429295758798</v>
-      </c>
-      <c r="G91">
-        <f t="shared" si="16"/>
-        <v>24.7899257033536</v>
-      </c>
-      <c r="H91">
-        <f t="shared" si="23"/>
+      <c r="D91" s="1">
         <v>7.6372642622761902</v>
       </c>
-      <c r="I91">
-        <f>D91+66</f>
+      <c r="E91" s="1">
         <v>73.500894617627949</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A92">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92" s="1">
+        <v>90</v>
+      </c>
+      <c r="B92" s="1">
         <v>49.779759778126703</v>
       </c>
-      <c r="B92">
+      <c r="C92" s="1">
         <v>10.324505303581001</v>
       </c>
-      <c r="C92">
-        <v>-6.5730463041181597</v>
-      </c>
-      <c r="D92">
-        <v>0.93842437610674101</v>
-      </c>
-      <c r="E92">
-        <v>90</v>
-      </c>
-      <c r="F92">
-        <f t="shared" si="15"/>
-        <v>49.779759778126703</v>
-      </c>
-      <c r="G92">
-        <f t="shared" si="16"/>
-        <v>10.324505303581001</v>
-      </c>
-      <c r="H92">
-        <f t="shared" si="23"/>
+      <c r="D92" s="1">
         <v>6.9269536958818403</v>
       </c>
-      <c r="I92">
-        <f>D92+76</f>
+      <c r="E92" s="1">
         <v>76.938424376106738</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A93">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93" s="1">
+        <v>91</v>
+      </c>
+      <c r="B93" s="1">
         <v>62.764108934769503</v>
       </c>
-      <c r="B93">
+      <c r="C93" s="1">
         <v>39.041479874653298</v>
       </c>
-      <c r="C93">
-        <v>-5.9028904825636896</v>
-      </c>
-      <c r="D93">
-        <v>1.9956331477290099</v>
-      </c>
-      <c r="E93">
-        <v>91</v>
-      </c>
-      <c r="F93">
-        <f t="shared" si="15"/>
-        <v>62.764108934769503</v>
-      </c>
-      <c r="G93">
-        <f t="shared" si="16"/>
-        <v>39.041479874653298</v>
-      </c>
-      <c r="H93">
-        <f t="shared" si="23"/>
+      <c r="D93" s="1">
         <v>7.5971095174363104</v>
       </c>
-      <c r="I93">
-        <f>D93+78</f>
+      <c r="E93" s="1">
         <v>79.995633147729009</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A94">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94" s="1">
+        <v>92</v>
+      </c>
+      <c r="B94" s="1">
         <v>58.977202865482703</v>
       </c>
-      <c r="B94">
+      <c r="C94" s="1">
         <v>30.866366479560899</v>
       </c>
-      <c r="C94">
-        <v>-6.9149379861875397</v>
-      </c>
-      <c r="D94">
-        <v>0.17123059651080599</v>
-      </c>
-      <c r="E94">
-        <v>92</v>
-      </c>
-      <c r="F94">
-        <f t="shared" si="15"/>
-        <v>58.977202865482703</v>
-      </c>
-      <c r="G94">
-        <f t="shared" si="16"/>
-        <v>30.866366479560899</v>
-      </c>
-      <c r="H94">
-        <f t="shared" si="23"/>
+      <c r="D94" s="1">
         <v>6.5850620138124603</v>
       </c>
-      <c r="I94">
-        <f>D94+68</f>
+      <c r="E94" s="1">
         <v>68.17123059651081</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A95">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A95" s="1">
+        <v>93</v>
+      </c>
+      <c r="B95" s="1">
         <v>55.5196080397684</v>
       </c>
-      <c r="B95">
+      <c r="C95" s="1">
         <v>33.381003941704002</v>
       </c>
-      <c r="C95">
-        <v>-5.5765841416716304</v>
-      </c>
-      <c r="D95">
-        <v>1.51332977340768</v>
-      </c>
-      <c r="E95">
-        <v>93</v>
-      </c>
-      <c r="F95">
-        <f t="shared" si="15"/>
-        <v>55.5196080397684</v>
-      </c>
-      <c r="G95">
-        <f t="shared" si="16"/>
-        <v>33.381003941704002</v>
-      </c>
-      <c r="H95">
-        <f t="shared" si="21"/>
+      <c r="D95" s="1">
         <v>4.4234158583283696</v>
       </c>
-      <c r="I95">
-        <f>D95+90</f>
+      <c r="E95" s="1">
         <v>91.513329773407676</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A96">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A96" s="1">
+        <v>94</v>
+      </c>
+      <c r="B96" s="1">
         <v>63.443294629692502</v>
       </c>
-      <c r="B96">
+      <c r="C96" s="1">
         <v>43.608208150891699</v>
       </c>
-      <c r="C96">
-        <v>-6.3141754726583104</v>
-      </c>
-      <c r="D96">
-        <v>-0.16074629973048099</v>
-      </c>
-      <c r="E96">
-        <v>94</v>
-      </c>
-      <c r="F96">
-        <f t="shared" si="15"/>
-        <v>63.443294629692502</v>
-      </c>
-      <c r="G96">
-        <f t="shared" si="16"/>
-        <v>43.608208150891699</v>
-      </c>
-      <c r="H96">
-        <f t="shared" si="21"/>
+      <c r="D96" s="1">
         <v>3.6858245273416896</v>
       </c>
-      <c r="I96">
-        <f>D96+88</f>
+      <c r="E96" s="1">
         <v>87.839253700269524</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A97">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A97" s="1">
+        <v>95</v>
+      </c>
+      <c r="B97" s="1">
         <v>64.827639474848596</v>
       </c>
-      <c r="B97">
+      <c r="C97" s="1">
         <v>5.04528302792842</v>
       </c>
-      <c r="C97">
-        <v>-5.4371373829664504</v>
-      </c>
-      <c r="D97">
-        <v>0.98439137740296501</v>
-      </c>
-      <c r="E97">
-        <v>95</v>
-      </c>
-      <c r="F97">
-        <f t="shared" si="15"/>
-        <v>64.827639474848596</v>
-      </c>
-      <c r="G97">
-        <f t="shared" si="16"/>
-        <v>5.04528302792842</v>
-      </c>
-      <c r="H97">
-        <f>SUM(C97,11.8)</f>
+      <c r="D97" s="1">
         <v>6.3628626170335503</v>
       </c>
-      <c r="I97">
-        <f>D97+88</f>
+      <c r="E97" s="1">
         <v>88.984391377402972</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A98">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A98" s="1">
+        <v>96</v>
+      </c>
+      <c r="B98" s="1">
         <v>52.999421348118197</v>
       </c>
-      <c r="B98">
+      <c r="C98" s="1">
         <v>63.9908127067254</v>
       </c>
-      <c r="C98">
-        <v>-6.0246576084970203</v>
-      </c>
-      <c r="D98">
-        <v>7.9425511309952596E-2</v>
-      </c>
-      <c r="E98">
-        <v>96</v>
-      </c>
-      <c r="F98">
-        <f t="shared" si="15"/>
-        <v>52.999421348118197</v>
-      </c>
-      <c r="G98">
-        <f t="shared" si="16"/>
-        <v>63.9908127067254</v>
-      </c>
-      <c r="H98">
-        <f t="shared" ref="H98:H101" si="24">SUM(C98,11.8)</f>
+      <c r="D98" s="1">
         <v>5.7753423915029805</v>
       </c>
-      <c r="I98">
-        <f>D98+93</f>
+      <c r="E98" s="1">
         <v>93.07942551130995</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A99">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A99" s="1">
+        <v>97</v>
+      </c>
+      <c r="B99" s="1">
         <v>49.695613054404902</v>
       </c>
-      <c r="B99">
+      <c r="C99" s="1">
         <v>5.9445113261559204</v>
       </c>
-      <c r="C99">
-        <v>-6.7006782059426504</v>
-      </c>
-      <c r="D99">
-        <v>1.71086022899379</v>
-      </c>
-      <c r="E99">
-        <v>97</v>
-      </c>
-      <c r="F99">
-        <f t="shared" si="15"/>
-        <v>49.695613054404902</v>
-      </c>
-      <c r="G99">
-        <f t="shared" si="16"/>
-        <v>5.9445113261559204</v>
-      </c>
-      <c r="H99">
-        <f t="shared" si="24"/>
+      <c r="D99" s="1">
         <v>5.0993217940573503</v>
       </c>
-      <c r="I99">
-        <f>D99+73</f>
+      <c r="E99" s="1">
         <v>74.710860228993795</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A100">
-        <v>155.721625773461</v>
-      </c>
-      <c r="B100">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A100" s="1">
+        <v>98</v>
+      </c>
+      <c r="B100" s="1">
+        <v>98.273650000000004</v>
+      </c>
+      <c r="C100" s="1">
         <v>22.341362182726101</v>
       </c>
-      <c r="C100">
-        <v>-6.5097546709390999</v>
-      </c>
-      <c r="D100">
-        <v>0.66517058711239996</v>
-      </c>
-      <c r="E100">
-        <v>98</v>
-      </c>
-      <c r="F100">
-        <f t="shared" si="15"/>
-        <v>155.721625773461</v>
-      </c>
-      <c r="G100">
-        <f t="shared" si="16"/>
-        <v>22.341362182726101</v>
-      </c>
-      <c r="H100">
-        <f t="shared" si="24"/>
+      <c r="D100" s="1">
         <v>5.2902453290609008</v>
       </c>
-      <c r="I100">
-        <f>D100+97</f>
+      <c r="E100" s="1">
         <v>97.665170587112399</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A101">
-        <v>148.091289730798</v>
-      </c>
-      <c r="B101">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A101" s="1">
+        <v>99</v>
+      </c>
+      <c r="B101" s="1">
+        <v>96.568929999999995</v>
+      </c>
+      <c r="C101" s="1">
         <v>20.5093403584446</v>
       </c>
-      <c r="C101">
-        <v>-5.6510849320307601</v>
-      </c>
-      <c r="D101">
-        <v>1.91904088315539</v>
-      </c>
-      <c r="E101">
-        <v>99</v>
-      </c>
-      <c r="F101">
-        <f t="shared" si="15"/>
-        <v>148.091289730798</v>
-      </c>
-      <c r="G101">
-        <f t="shared" si="16"/>
-        <v>20.5093403584446</v>
-      </c>
-      <c r="H101">
-        <f t="shared" si="24"/>
+      <c r="D101" s="1">
         <v>6.1489150679692406</v>
       </c>
-      <c r="I101">
-        <f>D101+76</f>
+      <c r="E101" s="1">
         <v>77.91904088315539</v>
       </c>
     </row>

</xml_diff>